<commit_message>
added power analysis and started website rework
</commit_message>
<xml_diff>
--- a/docs/data/sample-questions.xlsx
+++ b/docs/data/sample-questions.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lilia\Documents\R\01_paper\climate-crisis-behavior-sem\reports\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kojan\Documents\R\02_Publications\climate-crisis-behavior-sem\reports\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D017EF17-C61B-48C9-99E4-579E8121C6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="15600" xr2:uid="{4E106ECC-1413-479F-9D54-F609E084B0DA}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="15600"/>
   </bookViews>
   <sheets>
     <sheet name="sample-questions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -371,12 +370,6 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>(Rammstedt et al., 2020)</t>
-  </si>
-  <si>
-    <t>(Kovaleva et al., 2014)</t>
-  </si>
-  <si>
     <t>Extraversion*</t>
   </si>
   <si>
@@ -414,12 +407,18 @@
 more than 20,000 km
 don't know</t>
   </si>
+  <si>
+    <t>Rammstedt et al., 2020</t>
+  </si>
+  <si>
+    <t>Kovaleva et al., 2014</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -439,30 +438,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -470,36 +455,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -508,23 +468,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -836,22 +781,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE0834A-A0E4-4CFF-BC2A-4BBE2A8C38D5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26.83984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.26171875" customWidth="1"/>
+    <col min="3" max="3" width="30.68359375" customWidth="1"/>
     <col min="4" max="4" width="80" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -868,7 +813,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -876,7 +821,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -890,7 +835,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -904,7 +849,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -918,7 +863,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -932,7 +877,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -943,10 +888,10 @@
         <v>63</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -960,7 +905,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -974,7 +919,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -988,7 +933,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -996,7 +941,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -1010,7 +955,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -1024,7 +969,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -1038,7 +983,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -1049,10 +994,10 @@
         <v>75</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -1060,9 +1005,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B17" t="s">
         <v>30</v>
@@ -1073,11 +1018,11 @@
       <c r="D17" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
@@ -1090,13 +1035,13 @@
       <c r="D18" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B19" t="s">
         <v>34</v>
@@ -1107,11 +1052,11 @@
       <c r="D19" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
@@ -1124,11 +1069,11 @@
       <c r="D20" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
         <v>37</v>
       </c>
@@ -1141,11 +1086,11 @@
       <c r="D21" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
@@ -1158,13 +1103,13 @@
       <c r="D22" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B23" t="s">
         <v>40</v>
@@ -1175,13 +1120,13 @@
       <c r="D23" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B24" t="s">
         <v>41</v>
@@ -1192,11 +1137,11 @@
       <c r="D24" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -1209,13 +1154,13 @@
       <c r="D25" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B26" t="s">
         <v>43</v>
@@ -1226,11 +1171,11 @@
       <c r="D26" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -1243,11 +1188,11 @@
       <c r="D27" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
@@ -1260,11 +1205,11 @@
       <c r="D28" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
@@ -1277,13 +1222,13 @@
       <c r="D29" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E29" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B30" t="s">
         <v>47</v>
@@ -1294,11 +1239,11 @@
       <c r="D30" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E30" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -1311,11 +1256,11 @@
       <c r="D31" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -1328,11 +1273,11 @@
       <c r="D32" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -1345,11 +1290,11 @@
       <c r="D33" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E33" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -1362,11 +1307,11 @@
       <c r="D34" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E34" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -1379,16 +1324,11 @@
       <c r="D35" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E35" s="9" t="s">
-        <v>102</v>
+      <c r="E35" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E17:E18" location="Sources!A1" display="(Rammstedt et al., 2014)" xr:uid="{3B7DC1C5-59E9-487E-944B-87B5F66E11BB}"/>
-    <hyperlink ref="E32:E35" location="Sources!A1" display="(Kovaleva et al., 2014)" xr:uid="{D64FF086-E76C-4307-8E4E-440B11A59947}"/>
-    <hyperlink ref="E18:E31" location="Sources!A1" display="(Rammstedt et al., 2014)" xr:uid="{2C99A950-10CC-48C3-BFD7-8AD70019CA6B}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>